<commit_message>
sprint 100 manual testcases
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Outlet -Activity testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Outlet -Activity testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78019E34-B9CC-4679-80A1-18BFB25AA45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14575E47-D199-497D-9B8E-568DF2975E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>SL. No</t>
   </si>
@@ -550,6 +550,59 @@
   </si>
   <si>
     <t>It gets displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It displayed the name partiicular stock count tag column </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click the particular checkbox ,it shows the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Clear and Add tags" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and once click the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">'Add tags' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and type and save </t>
+    </r>
+  </si>
+  <si>
+    <t>Activity-&gt;check box(new)</t>
   </si>
 </sst>
 </file>
@@ -699,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -743,6 +796,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,6 +1460,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Manual testcases for Sprint 101 nd 102
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Outlet -Activity testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Outlet -Activity testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14575E47-D199-497D-9B8E-568DF2975E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AE8A5D-7B86-4855-9542-CF53E21772D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -552,7 +552,7 @@
     <t>It gets displayed</t>
   </si>
   <si>
-    <t xml:space="preserve">It displayed the name partiicular stock count tag column </t>
+    <t>Activity-&gt;check box(new)</t>
   </si>
   <si>
     <r>
@@ -598,11 +598,32 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">and type and save </t>
-    </r>
-  </si>
-  <si>
-    <t>Activity-&gt;check box(new)</t>
+      <t xml:space="preserve">and type and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Save</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>It displayed the name partiicular stock count tag column "Updated successfully"</t>
   </si>
 </sst>
 </file>
@@ -1083,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,13 +1492,13 @@
         <v>9</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>50</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>11</v>
@@ -1485,5 +1506,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sprint 108 MT cases
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Outlet -Activity testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Outlet -Activity testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F805D30-892C-4C06-8B59-B65063BB54F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F6132B-3828-456E-B765-0E2F65E58DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1104,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1144,7 +1144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Move to another inventory
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Outlet -Activity testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Outlet -Activity testcases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF17C14-BD90-42F9-8184-277BF908BA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EAF2A3-8DE3-4B7B-8F20-6ABE7F5BAE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
   <si>
     <t>SL. No</t>
   </si>
@@ -118,32 +118,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">It we take </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Adjustment record</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ,it will comse pop up on the Created date and name                                                                                                                                   1.Outlet, Reason, Item name, Inventory list, UOM, Quantity, Notes         2.If you click 'X' the returns back to Activity page                           </t>
-    </r>
-  </si>
-  <si>
     <t>It display the details of exact item</t>
   </si>
   <si>
@@ -198,8 +172,23 @@
     <t xml:space="preserve">After clicks the start stock count it goes to New stock count screen </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Select Outlet and Inventory and click Start stock count ,it goes to New </t>
+    <t>It dispalyed New stock count screen, SKU name search box, Name, Supplier, UOM, Last count, Counted, Qty and Save</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It displayed the SKU page </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Outlets-&gt;SKU-&gt; Record adjustment</t>
+  </si>
+  <si>
+    <t>By clicking Record adjustment ,it shows pop up screen "Outlet, Reason, Item name dropdown, Inventory list, UOM, Quantity, Notes and Save"</t>
+  </si>
+  <si>
+    <t>Activity-&gt;New stock count</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click the </t>
     </r>
     <r>
       <rPr>
@@ -210,251 +199,148 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>stock count page</t>
-    </r>
-  </si>
-  <si>
-    <t>It dispalyed New stock count screen, SKU name search box, Name, Supplier, UOM, Last count, Counted, Qty and Save</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It displayed the SKU page </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Outlets-&gt;SKU-&gt; Record adjustment</t>
-  </si>
-  <si>
-    <t>By clicking Record adjustment ,it shows pop up screen "Outlet, Reason, Item name dropdown, Inventory list, UOM, Quantity, Notes and Save"</t>
-  </si>
-  <si>
-    <t>Activity-&gt;New stock count</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Click the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t xml:space="preserve">Save button </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Save button </t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve">,it shows Update stock count? And </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">,it shows Update stock count? And </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>Save stock count</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Save stock count</t>
-    </r>
-    <r>
-      <rPr>
+      <t>,after clicking it returns back to Activity screen</t>
+    </r>
+  </si>
+  <si>
+    <t>Enter the required data and click Save button then it comes Successfully record added</t>
+  </si>
+  <si>
+    <t>If click the Export It will download the file                                                              *When exporting the data from this page we will include the 'Stock count corrections' in similar format to 'Adjustments'.</t>
+  </si>
+  <si>
+    <r>
+      <t>1.And search SKU and find the exact item                                                               2.Top right side</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Created by Buyer_Manual_01 date and Last updated date"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> will show the timestamp of the most recent amendment if any (new implementation)</t>
+    </r>
+  </si>
+  <si>
+    <t>It gets displayed</t>
+  </si>
+  <si>
+    <t>Activity-&gt;check box(new)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click the particular checkbox ,it shows the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,after clicking it returns back to Activity screen</t>
-    </r>
-  </si>
-  <si>
-    <t>Enter the required data and click Save button then it comes Successfully record added</t>
-  </si>
-  <si>
-    <t>If click the Export It will download the file                                                              *When exporting the data from this page we will include the 'Stock count corrections' in similar format to 'Adjustments'.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">It goes to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Stock count screen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in there "As of date and Est.value"                      1.How many items and SKU search box and Export</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.And search SKU and find the exact item                                                               2.Top right side</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Created by Buyer_Manual_01 date and Last updated date"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> will show the timestamp of the most recent amendment if any (new implementation)</t>
-    </r>
-  </si>
-  <si>
-    <t>If the qty has been amended, the value for the column is clickable and can show previously recorded quantities</t>
-  </si>
-  <si>
-    <t>It should display the 'History' pop up screen ,in there Date, User, Qty</t>
-  </si>
-  <si>
-    <r>
-      <t>There is a new</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF172B4D"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 'Stock count correction' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF172B4D"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>pop up screen detail page. It shows the previous qty and the amended qty.</t>
-    </r>
-  </si>
-  <si>
-    <t>It gets displayed</t>
-  </si>
-  <si>
-    <t>Activity-&gt;check box(new)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Click the particular checkbox ,it shows the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t xml:space="preserve">"Clear and Add tags" </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">"Clear and Add tags" </t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve">and once click the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">and once click the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t xml:space="preserve">'Add tags' </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">'Add tags' </t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve">and type and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">and type and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>Save</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Save</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
     <t>It displayed the name partiicular stock count tag column "Updated successfully"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">it shows pop up page </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Outlet dropdown, Inventory list dropdown, Count date (by default select the date) and start stock count</t>
-    </r>
   </si>
   <si>
     <r>
@@ -613,13 +499,97 @@
   </si>
   <si>
     <t>It gets displayed the select a List and Apply the Reset, Once click the Reset its clear the list</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It we take </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Adjustment record</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ,it will comse pop up on the Created date and name                                                                                                                                   1.Outlet, Reason, Item name, Inventory list, UOM, Quantity, Notes                     2.If you click 'X' the returns back to Activity page                           </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It goes to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Stock count screen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in there "As of date and Est.value"                      1.How many items and SKU search box, Add tags and Export</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">it shows pop up page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Outlet dropdown, Inventory list dropdown and start stock count</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select Outlet and Inventory and click Start stock count ,it goes to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New stock count page</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -681,19 +651,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF172B4D"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF172B4D"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -762,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -799,9 +756,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1085,23 +1039,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" customWidth="1"/>
-    <col min="5" max="5" width="63.5703125" customWidth="1"/>
-    <col min="6" max="6" width="52.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="3" max="3" width="33.81640625" customWidth="1"/>
+    <col min="4" max="4" width="48.1796875" customWidth="1"/>
+    <col min="5" max="5" width="63.54296875" customWidth="1"/>
+    <col min="6" max="6" width="52.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1141,16 +1095,16 @@
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1173,7 +1127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1184,16 +1138,16 @@
         <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1204,16 +1158,16 @@
         <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1227,7 +1181,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -1236,7 +1190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1250,7 +1204,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>15</v>
@@ -1259,7 +1213,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1273,16 +1227,16 @@
         <v>17</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1292,17 +1246,20 @@
       <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>37</v>
+      <c r="D9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1313,14 +1270,19 @@
         <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1330,20 +1292,20 @@
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>33</v>
+      <c r="D11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1353,20 +1315,20 @@
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="D12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1377,19 +1339,19 @@
         <v>9</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="43" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1400,19 +1362,19 @@
         <v>9</v>
       </c>
       <c r="D14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1422,62 +1384,16 @@
       <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>30</v>
+      <c r="D15" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="16" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>